<commit_message>
fix api export excel
</commit_message>
<xml_diff>
--- a/src/main/resources/template/BGGLG_EXCEL.xlsx
+++ b/src/main/resources/template/BGGLG_EXCEL.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ideiaProject\Bgglg\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BD75137-0F47-4C80-8CA6-FBC30C973ADF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Báo Cơm Hàng ngày" sheetId="2" r:id="rId1"/>
@@ -77,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -805,24 +804,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
-    <col min="4" max="5" width="16.25" style="3" customWidth="1"/>
-    <col min="6" max="18" width="8.25" style="3" customWidth="1"/>
+    <col min="4" max="5" width="16.19921875" style="3" customWidth="1"/>
+    <col min="6" max="18" width="8.19921875" style="3" customWidth="1"/>
     <col min="19" max="16384" width="13" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -844,7 +843,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -866,7 +865,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -888,7 +887,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -910,14 +909,14 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:18" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
@@ -945,7 +944,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -965,17 +964,17 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:18" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:14" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -987,8 +986,8 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1000,7 +999,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1012,7 +1011,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:14" s="5" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="5" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1024,8 +1023,8 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1040,7 +1039,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1055,7 +1054,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1070,7 +1069,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1085,7 +1084,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1100,7 +1099,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1115,7 +1114,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1130,7 +1129,7 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1145,7 +1144,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1160,7 +1159,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1175,7 +1174,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1190,7 +1189,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1205,7 +1204,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1220,7 +1219,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1235,7 +1234,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1250,7 +1249,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1265,7 +1264,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1280,7 +1279,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1295,7 +1294,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1310,7 +1309,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1325,7 +1324,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1340,7 +1339,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1355,7 +1354,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1370,7 +1369,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1385,7 +1384,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1400,7 +1399,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1415,7 +1414,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1430,7 +1429,7 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1445,7 +1444,7 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1460,7 +1459,7 @@
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1475,7 +1474,7 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1490,7 +1489,7 @@
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1505,7 +1504,7 @@
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1520,7 +1519,7 @@
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1535,7 +1534,7 @@
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -1550,7 +1549,7 @@
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1565,7 +1564,7 @@
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -1580,7 +1579,7 @@
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
     </row>
-    <row r="61" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -1595,7 +1594,7 @@
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
     </row>
-    <row r="62" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -1610,7 +1609,7 @@
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
     </row>
-    <row r="63" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -1625,7 +1624,7 @@
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -1640,7 +1639,7 @@
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -1655,7 +1654,7 @@
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
     </row>
-    <row r="66" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -1670,7 +1669,7 @@
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
     </row>
-    <row r="67" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -1685,7 +1684,7 @@
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
     </row>
-    <row r="68" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -1700,7 +1699,7 @@
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
     </row>
-    <row r="69" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -1715,7 +1714,7 @@
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -1730,7 +1729,7 @@
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -1745,7 +1744,7 @@
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -1760,7 +1759,7 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -1775,7 +1774,7 @@
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
     </row>
-    <row r="74" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -1790,7 +1789,7 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -1805,7 +1804,7 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -1820,7 +1819,7 @@
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
     </row>
-    <row r="77" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -1835,7 +1834,7 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -1850,7 +1849,7 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -1865,7 +1864,7 @@
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -1880,7 +1879,7 @@
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
     </row>
-    <row r="81" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -1895,7 +1894,7 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -1910,7 +1909,7 @@
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -1925,7 +1924,7 @@
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
     </row>
-    <row r="84" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -1940,7 +1939,7 @@
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
     </row>
-    <row r="85" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -1971,24 +1970,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
-    <col min="4" max="5" width="16.25" style="3" customWidth="1"/>
-    <col min="6" max="18" width="8.25" style="3" customWidth="1"/>
+    <col min="4" max="5" width="16.19921875" style="3" customWidth="1"/>
+    <col min="6" max="18" width="8.19921875" style="3" customWidth="1"/>
     <col min="19" max="16384" width="13" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2010,7 +2009,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2032,7 +2031,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -2054,7 +2053,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
@@ -2076,14 +2075,14 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
@@ -2113,7 +2112,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -2150,24 +2149,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="30.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
-    <col min="4" max="5" width="16.25" style="3" customWidth="1"/>
-    <col min="6" max="18" width="8.25" style="3" customWidth="1"/>
+    <col min="4" max="5" width="16.19921875" style="3" customWidth="1"/>
+    <col min="6" max="18" width="8.19921875" style="3" customWidth="1"/>
     <col min="19" max="16384" width="13" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2189,7 +2188,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2211,7 +2210,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -2233,7 +2232,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -2255,14 +2254,14 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
@@ -2292,7 +2291,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="14"/>
       <c r="C7" s="19"/>

</xml_diff>